<commit_message>
Self assessment document, done!
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolas\IdeaProjects\lapr3-2021-g129\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maiad\IdeaProjects\lapr3-2021-g129\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32387B2C-2F10-4777-8088-C99AC752B698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6508E126-87AC-4273-90E5-74249D0E92B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
     <sheet name="User Stories" sheetId="5" r:id="rId2"/>
-    <sheet name="Code Quality" sheetId="8" r:id="rId3"/>
-    <sheet name="Project Development" sheetId="1" r:id="rId4"/>
+    <sheet name="Project Development" sheetId="1" r:id="rId3"/>
+    <sheet name="Code Quality" sheetId="8" r:id="rId4"/>
     <sheet name="Project Management" sheetId="10" r:id="rId5"/>
     <sheet name="Physics" sheetId="9" r:id="rId6"/>
   </sheets>
@@ -587,7 +587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,6 +639,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1148,7 +1156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1386,6 +1394,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2082,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2324,10 +2338,18 @@
       <c r="C13" s="8">
         <v>1191419</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="39"/>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9">
+        <v>5</v>
+      </c>
+      <c r="G13" s="39">
+        <v>5</v>
+      </c>
       <c r="H13" s="38"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -2339,9 +2361,9 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="54" t="e">
+      <c r="S13" s="54">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2355,7 +2377,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="39"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="85"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -2765,7 +2787,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2773,7 +2796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2873,8 +2898,12 @@
       <c r="A6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="8">
+        <v>1190718</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="34" t="s">
         <v>39</v>
@@ -2899,8 +2928,12 @@
       <c r="A7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8">
+        <v>1190782</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5</v>
+      </c>
       <c r="D7" s="13"/>
       <c r="E7" s="15" t="s">
         <v>39</v>
@@ -2925,8 +2958,12 @@
       <c r="A8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="8">
+        <v>1190811</v>
+      </c>
+      <c r="C8" s="8">
+        <v>5</v>
+      </c>
       <c r="D8" s="13"/>
       <c r="E8" s="15" t="s">
         <v>39</v>
@@ -2951,8 +2988,12 @@
       <c r="A9" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="8">
+        <v>1190718</v>
+      </c>
+      <c r="C9" s="8">
+        <v>5</v>
+      </c>
       <c r="D9" s="13"/>
       <c r="E9" s="15" t="s">
         <v>39</v>
@@ -2977,8 +3018,12 @@
       <c r="A10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="8">
+        <v>1190782</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
       <c r="D10" s="13"/>
       <c r="E10" s="15" t="s">
         <v>39</v>
@@ -3003,8 +3048,12 @@
       <c r="A11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="8">
+        <v>1191419</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
       <c r="D11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>39</v>
@@ -3029,8 +3078,12 @@
       <c r="A12" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="8">
+        <v>1191419</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
       <c r="D12" s="13"/>
       <c r="E12" s="15" t="s">
         <v>39</v>
@@ -3057,7 +3110,7 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="86"/>
       <c r="E13" s="15" t="s">
         <v>39</v>
       </c>
@@ -3490,153 +3543,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B77AED-41D5-8047-A901-AF6E531ADCF8}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="6" width="14.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="11">
-        <v>34</v>
-      </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="22">
-        <v>80</v>
-      </c>
-      <c r="E4" s="22">
-        <v>90</v>
-      </c>
-      <c r="F4" s="12">
-        <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
-        <v>-800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="15">
-        <v>21</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="7">
-        <v>75</v>
-      </c>
-      <c r="E5" s="7">
-        <v>85</v>
-      </c>
-      <c r="F5" s="16">
-        <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>-750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="15">
-        <v>-13</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="7">
-        <v>5</v>
-      </c>
-      <c r="E6" s="7">
-        <v>10</v>
-      </c>
-      <c r="F6" s="16">
-        <f>(IF((D6-C6)*10*-1*2&gt;100,100,IF((((D6-C6)*10*-1*2))&lt;0,0,(D6-C6)*10*-1*2)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="23">
-        <v>-13</v>
-      </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="24">
-        <v>5</v>
-      </c>
-      <c r="E7" s="24">
-        <v>10</v>
-      </c>
-      <c r="F7" s="17">
-        <f>(IF((D7-C7)*10*-1*2&gt;100,100,IF((((D7-C7)*10*-1*2))&lt;0,0,(D7-C7)*10*-1*2)))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="57">
-        <v>55</v>
-      </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58">
-        <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>-429.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="69">
-        <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20984BA6-2128-EB41-A750-F94245E6A6D5}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
@@ -3789,67 +3695,67 @@
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>0</v>
+        <v>4.3127272727272734</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>75</v>
@@ -4070,63 +3976,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5094545454545456</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4145,63 +4051,63 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.0378181818181815</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -4229,12 +4135,169 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B77AED-41D5-8047-A901-AF6E531ADCF8}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="6" width="14.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="11">
+        <v>34</v>
+      </c>
+      <c r="C4" s="64">
+        <v>90.7</v>
+      </c>
+      <c r="D4" s="22">
+        <v>80</v>
+      </c>
+      <c r="E4" s="22">
+        <v>90</v>
+      </c>
+      <c r="F4" s="12">
+        <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="15">
+        <v>21</v>
+      </c>
+      <c r="C5" s="31">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="D5" s="7">
+        <v>75</v>
+      </c>
+      <c r="E5" s="7">
+        <v>85</v>
+      </c>
+      <c r="F5" s="16">
+        <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
+        <v>64.000000000000057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="15">
+        <v>-13</v>
+      </c>
+      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16">
+        <f>(IF((D6-C6)*10*-1*2&gt;100,100,IF((((D6-C6)*10*-1*2))&lt;0,0,(D6-C6)*10*-1*2)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="23">
+        <v>-13</v>
+      </c>
+      <c r="C7" s="65">
+        <v>3</v>
+      </c>
+      <c r="D7" s="24">
+        <v>5</v>
+      </c>
+      <c r="E7" s="24">
+        <v>10</v>
+      </c>
+      <c r="F7" s="17">
+        <f>(IF((D7-C7)*10*-1*2&gt;100,100,IF((((D7-C7)*10*-1*2))&lt;0,0,(D7-C7)*10*-1*2)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="57">
+        <v>55</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58">
+        <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
+        <v>47.440000000000012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="69">
+        <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
+        <v>0.86254545454545473</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5251,18 +5314,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5284,14 +5347,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5305,4 +5360,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>